<commit_message>
Monster rooms now have custom coloured text.
Level layout was also changed slightly.
</commit_message>
<xml_diff>
--- a/TextAdventure/Level.xlsx
+++ b/TextAdventure/Level.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack.buscumbvi\Documents\Assessments\TextAdventure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack.buscumbvi\Documents\Assessments\AIE-Assessment-1-Intro-to-CPP\TextAdventure\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="3">
   <si>
     <t>Start</t>
   </si>
@@ -112,7 +112,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -145,6 +145,43 @@
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
@@ -158,25 +195,40 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -464,141 +516,145 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="7"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5"/>
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="1"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="2"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="1"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="7"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="7"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="1"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="2"/>
       <c r="B11" s="3"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="2"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="1"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="2"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="D13:D15"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
@@ -613,11 +669,11 @@
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>